<commit_message>
Gathering and sorting the results from the tests
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vicuyzb\source\repos\python_stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8299D42-0BDD-4493-B627-74C160B941BD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382DAACB-108B-4C73-A52C-30CEBE12C892}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9F6B9CB7-5928-4F67-A075-287239088E00}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="330" xr2:uid="{9F6B9CB7-5928-4F67-A075-287239088E00}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Results" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
   <si>
     <t>Common</t>
   </si>
@@ -49,12 +49,40 @@
   </si>
   <si>
     <t>5000 incidents</t>
+  </si>
+  <si>
+    <t>10000 incidents</t>
+  </si>
+  <si>
+    <t>15000 incidents</t>
+  </si>
+  <si>
+    <t>20000 incidents</t>
+  </si>
+  <si>
+    <t>2k</t>
+  </si>
+  <si>
+    <t>5k</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>Words</t>
+  </si>
+  <si>
+    <t>Percentage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -79,15 +107,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -95,28 +135,68 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -429,146 +509,610 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D768AEE-202D-4FE9-93F0-4109FFCDB8C0}">
-  <dimension ref="A1:E9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{908D846E-C19D-4449-8B9B-6B4CC78D859B}">
+  <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="4"/>
-    <col min="3" max="3" width="9.140625" style="7"/>
-    <col min="4" max="4" width="9.140625" style="4"/>
-    <col min="5" max="5" width="9.140625" style="7"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="17"/>
+      <c r="E1" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="18"/>
+      <c r="G1" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="17"/>
+      <c r="I1" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="18"/>
+      <c r="K1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="17"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4">
+      <c r="C3" s="8">
+        <v>57942</v>
+      </c>
+      <c r="D3" s="9">
+        <f>C3/(C$3+C$4)</f>
+        <v>0.48746056450595215</v>
+      </c>
+      <c r="E3" s="10">
+        <v>63049</v>
+      </c>
+      <c r="F3" s="11">
+        <f>E3/(E$3+E$4)</f>
+        <v>0.53042527236781223</v>
+      </c>
+      <c r="G3" s="8">
+        <v>70912</v>
+      </c>
+      <c r="H3" s="9">
+        <f>G3/(G$3+G$4)</f>
+        <v>0.59657594750347032</v>
+      </c>
+      <c r="I3" s="10">
+        <v>78298</v>
+      </c>
+      <c r="J3" s="11">
+        <f>I3/(I$3+I$4)</f>
+        <v>0.65871366676481724</v>
+      </c>
+      <c r="K3" s="8">
         <v>81050</v>
       </c>
-      <c r="C3" s="6">
-        <f>B3/($B$3+$B$4)</f>
+      <c r="L3" s="9">
+        <f>K3/(K$3+K$4)</f>
         <v>0.68186598241702767</v>
       </c>
-      <c r="D3" s="5">
-        <v>57942</v>
-      </c>
-      <c r="E3" s="6">
-        <f>D3/($D$3+$D$4)</f>
-        <v>0.48746056450595215</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4">
+      <c r="C4" s="8">
+        <v>60923</v>
+      </c>
+      <c r="D4" s="9">
+        <f>C4/(C$3+C$4)</f>
+        <v>0.5125394354940479</v>
+      </c>
+      <c r="E4" s="10">
+        <v>55816</v>
+      </c>
+      <c r="F4" s="11">
+        <f>E4/(E$3+E$4)</f>
+        <v>0.46957472763218777</v>
+      </c>
+      <c r="G4" s="8">
+        <v>47953</v>
+      </c>
+      <c r="H4" s="9">
+        <f>G4/(G$3+G$4)</f>
+        <v>0.40342405249652968</v>
+      </c>
+      <c r="I4" s="10">
+        <v>40567</v>
+      </c>
+      <c r="J4" s="11">
+        <f>I4/(I$3+I$4)</f>
+        <v>0.34128633323518276</v>
+      </c>
+      <c r="K4" s="8">
         <v>37815</v>
       </c>
-      <c r="C4" s="6">
-        <f>B4/($B$3+$B$4)</f>
+      <c r="L4" s="9">
+        <f>K4/(K$3+K$4)</f>
         <v>0.31813401758297227</v>
       </c>
-      <c r="D4" s="5">
-        <v>60923</v>
-      </c>
-      <c r="E4" s="6">
-        <f>D4/($D$3+$D$4)</f>
-        <v>0.5125394354940479</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="B5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="8">
-        <v>412542</v>
-      </c>
-      <c r="C8" s="6">
-        <f>B8/($B$8+$B$9)</f>
-        <v>0.67714090154799167</v>
+      <c r="C5" s="8">
+        <v>234543</v>
+      </c>
+      <c r="D5" s="9">
+        <f>C5/(C$5+C$6)</f>
+        <v>0.48505698633196631</v>
+      </c>
+      <c r="E5" s="10">
+        <v>256107</v>
+      </c>
+      <c r="F5" s="11">
+        <f>E5/(E$5+E$6)</f>
+        <v>0.52965336675373342</v>
+      </c>
+      <c r="G5" s="8">
+        <v>288184</v>
+      </c>
+      <c r="H5" s="9">
+        <f>G5/(G$5+G$6)</f>
+        <v>0.59599162008284789</v>
+      </c>
+      <c r="I5" s="10">
+        <v>316437</v>
+      </c>
+      <c r="J5" s="11">
+        <f>I5/(I$5+I$6)</f>
+        <v>0.65442148170667391</v>
+      </c>
+      <c r="K5" s="8">
+        <v>327791</v>
+      </c>
+      <c r="L5" s="9">
+        <f>K5/(K$5+K$6)</f>
+        <v>0.67790262172284643</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="8">
+        <v>248994</v>
+      </c>
+      <c r="D6" s="9">
+        <f>C6/(C$5+C$6)</f>
+        <v>0.51494301366803363</v>
+      </c>
+      <c r="E6" s="10">
+        <v>227430</v>
+      </c>
+      <c r="F6" s="11">
+        <f>E6/(E$5+E$6)</f>
+        <v>0.47034663324626658</v>
+      </c>
+      <c r="G6" s="8">
+        <v>195353</v>
+      </c>
+      <c r="H6" s="9">
+        <f>G6/(G$5+G$6)</f>
+        <v>0.40400837991715216</v>
+      </c>
+      <c r="I6" s="10">
+        <v>167100</v>
+      </c>
+      <c r="J6" s="11">
+        <f>I6/(I$5+I$6)</f>
+        <v>0.34557851829332603</v>
+      </c>
+      <c r="K6" s="8">
+        <v>155746</v>
+      </c>
+      <c r="L6" s="9">
+        <f>K6/(K$5+K$6)</f>
+        <v>0.32209737827715357</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="8">
+        <v>353968</v>
+      </c>
+      <c r="D7" s="9">
+        <f>C7/(C$7+C$8)</f>
+        <v>0.48249042088145611</v>
+      </c>
+      <c r="E7" s="10">
+        <v>386884</v>
+      </c>
+      <c r="F7" s="11">
+        <f>E7/(E$7+E$8)</f>
+        <v>0.52735790803773575</v>
+      </c>
+      <c r="G7" s="8">
+        <v>435737</v>
+      </c>
+      <c r="H7" s="9">
+        <f>G7/(G$7+G$8)</f>
+        <v>0.59394896861756719</v>
+      </c>
+      <c r="I7" s="10">
+        <v>477807</v>
+      </c>
+      <c r="J7" s="11">
+        <f>I7/(I$7+I$8)</f>
+        <v>0.65129418628267499</v>
+      </c>
+      <c r="K7" s="8">
+        <v>495005</v>
+      </c>
+      <c r="L7" s="9">
+        <f>K7/(K$7+K$8)</f>
+        <v>0.67473661683662134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="8">
+        <v>379659</v>
       </c>
       <c r="D8" s="9">
-        <v>294936</v>
-      </c>
-      <c r="E8" s="6">
-        <f>D8/($D$8+$D$9)</f>
-        <v>0.48410399168801838</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+        <f>C8/(C$7+C$8)</f>
+        <v>0.51750957911854389</v>
+      </c>
+      <c r="E8" s="10">
+        <v>346743</v>
+      </c>
+      <c r="F8" s="11">
+        <f>E8/(E$7+E$8)</f>
+        <v>0.4726420919622642</v>
+      </c>
+      <c r="G8" s="8">
+        <v>297890</v>
+      </c>
+      <c r="H8" s="9">
+        <f>G8/(G$7+G$8)</f>
+        <v>0.40605103138243276</v>
+      </c>
+      <c r="I8" s="10">
+        <v>255820</v>
+      </c>
+      <c r="J8" s="11">
+        <f>I8/(I$7+I$8)</f>
+        <v>0.34870581371732501</v>
+      </c>
+      <c r="K8" s="8">
+        <v>238622</v>
+      </c>
+      <c r="L8" s="9">
+        <f>K8/(K$7+K$8)</f>
+        <v>0.32526338316337866</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="8">
+        <v>537975</v>
+      </c>
+      <c r="D9" s="9">
+        <f>C9/(C$9+C$10)</f>
+        <v>0.47874427905147277</v>
+      </c>
+      <c r="E9" s="10">
+        <v>588205</v>
+      </c>
+      <c r="F9" s="11">
+        <f>E9/(E$9+E$10)</f>
+        <v>0.52344398654114321</v>
+      </c>
+      <c r="G9" s="8">
+        <v>663409</v>
+      </c>
+      <c r="H9" s="9">
+        <f>G9/(G$9+G$10)</f>
+        <v>0.59036807179006179</v>
+      </c>
+      <c r="I9" s="10">
+        <v>726463</v>
+      </c>
+      <c r="J9" s="11">
+        <f>I9/(I$9+I$10)</f>
+        <v>0.64647986466391572</v>
+      </c>
+      <c r="K9" s="8">
+        <v>752930</v>
+      </c>
+      <c r="L9" s="9">
+        <f>K9/(K$9+K$10)</f>
+        <v>0.67003286402941653</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+      <c r="B10" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="8">
-        <v>196699</v>
-      </c>
-      <c r="C9" s="6">
-        <f>B9/($B$8+$B$9)</f>
-        <v>0.32285909845200833</v>
-      </c>
-      <c r="D9" s="9">
-        <v>314305</v>
-      </c>
-      <c r="E9" s="6">
-        <f>D9/($D$8+$D$9)</f>
-        <v>0.51589600831198168</v>
+      <c r="C10" s="8">
+        <v>585746</v>
+      </c>
+      <c r="D10" s="9">
+        <f>C10/(C$9+C$10)</f>
+        <v>0.52125572094852723</v>
+      </c>
+      <c r="E10" s="10">
+        <v>535516</v>
+      </c>
+      <c r="F10" s="11">
+        <f>E10/(E$9+E$10)</f>
+        <v>0.47655601345885679</v>
+      </c>
+      <c r="G10" s="8">
+        <v>460312</v>
+      </c>
+      <c r="H10" s="9">
+        <f>G10/(G$9+G$10)</f>
+        <v>0.40963192820993821</v>
+      </c>
+      <c r="I10" s="10">
+        <v>397258</v>
+      </c>
+      <c r="J10" s="11">
+        <f>I10/(I$9+I$10)</f>
+        <v>0.35352013533608434</v>
+      </c>
+      <c r="K10" s="8">
+        <v>370791</v>
+      </c>
+      <c r="L10" s="9">
+        <f>K10/(K$9+K$10)</f>
+        <v>0.32996713597058347</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="8">
+        <v>656707</v>
+      </c>
+      <c r="D11" s="9">
+        <f>C11/(C$11+C$12)</f>
+        <v>0.48044196971060393</v>
+      </c>
+      <c r="E11" s="10">
+        <v>717995</v>
+      </c>
+      <c r="F11" s="11">
+        <f>E11/(E$11+E$12)</f>
+        <v>0.52527981587277894</v>
+      </c>
+      <c r="G11" s="8">
+        <v>809832</v>
+      </c>
+      <c r="H11" s="9">
+        <f>G11/(G$11+G$12)</f>
+        <v>0.59246708382075686</v>
+      </c>
+      <c r="I11" s="10">
+        <v>886581</v>
+      </c>
+      <c r="J11" s="11">
+        <f>I11/(I$11+I$12)</f>
+        <v>0.64861608289236594</v>
+      </c>
+      <c r="K11" s="8">
+        <v>918835</v>
+      </c>
+      <c r="L11" s="9">
+        <f>K11/(K$11+K$12)</f>
+        <v>0.67221287003038299</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
+      <c r="B12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="8">
+        <v>710174</v>
+      </c>
+      <c r="D12" s="9">
+        <f>C12/(C$11+C$12)</f>
+        <v>0.51955803028939607</v>
+      </c>
+      <c r="E12" s="10">
+        <v>648886</v>
+      </c>
+      <c r="F12" s="11">
+        <f>E12/(E$11+E$12)</f>
+        <v>0.474720184127221</v>
+      </c>
+      <c r="G12" s="8">
+        <v>557049</v>
+      </c>
+      <c r="H12" s="9">
+        <f>G12/(G$11+G$12)</f>
+        <v>0.40753291617924309</v>
+      </c>
+      <c r="I12" s="10">
+        <v>480300</v>
+      </c>
+      <c r="J12" s="11">
+        <f>I12/(I$11+I$12)</f>
+        <v>0.35138391710763411</v>
+      </c>
+      <c r="K12" s="8">
+        <v>448046</v>
+      </c>
+      <c r="L12" s="9">
+        <f>K12/(K$11+K$12)</f>
+        <v>0.32778712996961695</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="13"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="13"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="15">
+        <f>AVERAGE(D3,D5,D7,D9,D11)</f>
+        <v>0.48283884409629019</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="15">
+        <f>AVERAGE(F3,F5,F7,F9,F11)</f>
+        <v>0.52723206991464067</v>
+      </c>
+      <c r="G15" s="14"/>
+      <c r="H15" s="15">
+        <f>AVERAGE(H3,H5,H7,H9,H11)</f>
+        <v>0.59387033836294079</v>
+      </c>
+      <c r="I15" s="14"/>
+      <c r="J15" s="15">
+        <f>AVERAGE(J3,J5,J7,J9,J11)</f>
+        <v>0.65190505646208963</v>
+      </c>
+      <c r="K15" s="14"/>
+      <c r="L15" s="15">
+        <f>AVERAGE(L3,L5,L7,L9,L11)</f>
+        <v>0.6753501910072589</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="15">
+        <f>AVERAGE(D4,D6,D8,D10,D12)</f>
+        <v>0.51716115590370981</v>
+      </c>
+      <c r="E16" s="14"/>
+      <c r="F16" s="15">
+        <f>AVERAGE(F4,F6,F8,F10,F12)</f>
+        <v>0.47276793008535928</v>
+      </c>
+      <c r="G16" s="14"/>
+      <c r="H16" s="15">
+        <f>AVERAGE(H4,H6,H8,H10,H12)</f>
+        <v>0.40612966163705916</v>
+      </c>
+      <c r="I16" s="14"/>
+      <c r="J16" s="15">
+        <f>AVERAGE(J4,J6,J8,J10,J12)</f>
+        <v>0.34809494353791048</v>
+      </c>
+      <c r="K16" s="14"/>
+      <c r="L16" s="15">
+        <f>AVERAGE(L4,L6,L8,L10,L12)</f>
+        <v>0.32464980899274098</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
+  <mergeCells count="10">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="C1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating part of the new results
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vicuyzb\source\repos\python_stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382DAACB-108B-4C73-A52C-30CEBE12C892}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE503909-004E-46C0-979E-F56DC9AD9F98}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="330" xr2:uid="{9F6B9CB7-5928-4F67-A075-287239088E00}"/>
   </bookViews>
@@ -107,7 +107,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -123,6 +123,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -156,7 +162,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -185,6 +191,8 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -512,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{908D846E-C19D-4449-8B9B-6B4CC78D859B}">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,26 +543,26 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="18" t="s">
+      <c r="D1" s="19"/>
+      <c r="E1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="17" t="s">
+      <c r="F1" s="20"/>
+      <c r="G1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="I1" s="18" t="s">
+      <c r="H1" s="19"/>
+      <c r="I1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="18"/>
-      <c r="K1" s="17" t="s">
+      <c r="J1" s="20"/>
+      <c r="K1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="17"/>
+      <c r="L1" s="19"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -591,18 +599,18 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="18" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="8">
-        <v>57942</v>
-      </c>
-      <c r="D3" s="9">
+      <c r="C3" s="16">
+        <v>681</v>
+      </c>
+      <c r="D3" s="17">
         <f>C3/(C$3+C$4)</f>
-        <v>0.48746056450595215</v>
+        <v>0.10535272277227722</v>
       </c>
       <c r="E3" s="10">
         <v>63049</v>
@@ -634,16 +642,16 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="8">
-        <v>60923</v>
-      </c>
-      <c r="D4" s="9">
+      <c r="C4" s="16">
+        <v>5783</v>
+      </c>
+      <c r="D4" s="17">
         <f>C4/(C$3+C$4)</f>
-        <v>0.5125394354940479</v>
+        <v>0.89464727722772275</v>
       </c>
       <c r="E4" s="10">
         <v>55816</v>
@@ -675,7 +683,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="18" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -718,7 +726,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="7" t="s">
         <v>1</v>
       </c>
@@ -759,7 +767,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="18" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -802,7 +810,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="7" t="s">
         <v>1</v>
       </c>
@@ -843,7 +851,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="18" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -886,7 +894,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="7" t="s">
         <v>1</v>
       </c>
@@ -927,7 +935,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -970,7 +978,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="7" t="s">
         <v>1</v>
       </c>
@@ -1046,7 +1054,7 @@
       <c r="C15" s="14"/>
       <c r="D15" s="15">
         <f>AVERAGE(D3,D5,D7,D9,D11)</f>
-        <v>0.48283884409629019</v>
+        <v>0.40641727574955533</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="15">
@@ -1077,7 +1085,7 @@
       <c r="C16" s="14"/>
       <c r="D16" s="15">
         <f>AVERAGE(D4,D6,D8,D10,D12)</f>
-        <v>0.51716115590370981</v>
+        <v>0.59358272425044467</v>
       </c>
       <c r="E16" s="14"/>
       <c r="F16" s="15">

</xml_diff>

<commit_message>
Adding the results for 100k incidents to the table and graph.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vicuyzb\source\repos\python_stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE5EE79-9127-4364-A1D7-999D8FC1E9F5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52C4B0F-DD28-4A4A-81A8-0B0B20C563B5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-4110" windowWidth="19440" windowHeight="15000" tabRatio="330" activeTab="1" xr2:uid="{9F6B9CB7-5928-4F67-A075-287239088E00}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="13">
   <si>
     <t>Common</t>
   </si>
@@ -105,7 +105,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -127,6 +127,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -160,7 +166,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -190,18 +196,23 @@
     <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="10" fontId="2" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -363,9 +374,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1k</c:v>
                 </c:pt>
@@ -383,16 +394,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>50k</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100k</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$7</c:f>
+              <c:f>Sheet1!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.89464727722772275</c:v>
                 </c:pt>
@@ -410,6 +424,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.9896887138482845</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99334061060421941</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -473,9 +490,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1k</c:v>
                 </c:pt>
@@ -493,16 +510,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>50k</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100k</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$7</c:f>
+              <c:f>Sheet1!$C$2:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.10535272277227722</c:v>
                 </c:pt>
@@ -520,6 +540,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.0311286151715482E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.6593893957805558E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1747,7 +1770,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1771,32 +1794,32 @@
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="17" t="s">
+      <c r="E1" s="19"/>
+      <c r="F1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="18" t="s">
+      <c r="G1" s="20"/>
+      <c r="H1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="18"/>
-      <c r="J1" s="17" t="s">
+      <c r="I1" s="19"/>
+      <c r="J1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="17"/>
-      <c r="L1" s="18" t="s">
+      <c r="K1" s="20"/>
+      <c r="L1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="18"/>
+      <c r="M1" s="19"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="17" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="2"/>
@@ -1832,7 +1855,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="7" t="str">
@@ -1871,7 +1894,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="7" t="str">
         <f>A$3&amp;" Inc (NC)"</f>
         <v>1k Inc (NC)</v>
@@ -1908,7 +1931,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="7" t="str">
@@ -1947,7 +1970,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="7" t="str">
         <f>A$5&amp;" Inc (NC)"</f>
         <v>2k Inc (NC)</v>
@@ -1984,7 +2007,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="7" t="str">
@@ -2023,7 +2046,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="7" t="str">
         <f>A$7&amp;" Inc (NC)"</f>
         <v>5k Inc (NC)</v>
@@ -2060,7 +2083,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="7" t="str">
@@ -2099,7 +2122,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="7" t="str">
         <f>A$9&amp;" Inc (NC)"</f>
         <v>10k Inc (NC)</v>
@@ -2136,7 +2159,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="18" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="7" t="str">
@@ -2175,7 +2198,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="7" t="str">
         <f>A$11&amp;" Inc (NC)"</f>
         <v>20k Inc (NC)</v>
@@ -2212,7 +2235,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="18" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="7" t="str">
@@ -2251,7 +2274,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
+      <c r="A14" s="18"/>
       <c r="B14" s="7" t="str">
         <f>A$13&amp;" Inc (NC)"</f>
         <v>50k Inc (NC)</v>
@@ -2288,7 +2311,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="18" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="7" t="str">
@@ -2298,8 +2321,13 @@
       <c r="C15" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="9"/>
+      <c r="D15" s="8">
+        <v>970</v>
+      </c>
+      <c r="E15" s="9">
+        <f>D15/(D$15+D$16)</f>
+        <v>6.6593893957805558E-3</v>
+      </c>
       <c r="F15" s="10"/>
       <c r="G15" s="9" t="e">
         <f>F15/(F$15+F$16)</f>
@@ -2322,7 +2350,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="7" t="str">
         <f>A$15&amp;" Inc (NC)"</f>
         <v>100k Inc (NC)</v>
@@ -2330,8 +2358,13 @@
       <c r="C16" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="9"/>
+      <c r="D16" s="8">
+        <v>144689</v>
+      </c>
+      <c r="E16" s="9">
+        <f>D16/(D$15+D$16)</f>
+        <v>0.99334061060421941</v>
+      </c>
       <c r="F16" s="10"/>
       <c r="G16" s="9" t="e">
         <f>F16/(F$15+F$16)</f>
@@ -2377,7 +2410,7 @@
       <c r="D18" s="13"/>
       <c r="E18" s="14">
         <f>AVERAGE(E3,E5,E7,E9,E11,E13,E15)</f>
-        <v>4.6785186767401871E-2</v>
+        <v>4.1052930000027396E-2</v>
       </c>
       <c r="F18" s="13"/>
       <c r="G18" s="14" t="e">
@@ -2409,7 +2442,7 @@
       <c r="D19" s="13"/>
       <c r="E19" s="14">
         <f>AVERAGE(E4,E6,E8,E10,E12,E14,E16)</f>
-        <v>0.95321481323259816</v>
+        <v>0.95894706999997259</v>
       </c>
       <c r="F19" s="13"/>
       <c r="G19" s="14" t="e">
@@ -2434,18 +2467,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="A3:A4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2454,27 +2487,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32844F55-7C7E-4805-B0B9-974AE66C65D5}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="21" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2482,10 +2515,10 @@
       <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="23">
         <v>0.89464727722772275</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="22">
         <v>0.10535272277227722</v>
       </c>
     </row>
@@ -2493,10 +2526,10 @@
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="23">
         <v>0.92582524271844657</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="22">
         <v>7.41747572815534E-2</v>
       </c>
     </row>
@@ -2504,10 +2537,10 @@
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="23">
         <v>0.95620671283963776</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="22">
         <v>4.3793287160362279E-2</v>
       </c>
     </row>
@@ -2515,10 +2548,10 @@
       <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="23">
         <v>0.97182507664999196</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="22">
         <v>2.8174923350008069E-2</v>
       </c>
     </row>
@@ -2526,10 +2559,10 @@
       <c r="A6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="23">
         <v>0.98109585611150518</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="22">
         <v>1.8904143888494762E-2</v>
       </c>
     </row>
@@ -2537,11 +2570,22 @@
       <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="23">
         <v>0.9896887138482845</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="22">
         <v>1.0311286151715482E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="23">
+        <v>0.99334061060421941</v>
+      </c>
+      <c r="C8" s="22">
+        <v>6.6593893957805558E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gathering results from tests.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vicuyzb\source\repos\python_stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52C4B0F-DD28-4A4A-81A8-0B0B20C563B5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5E32A2-ABC2-4543-8A1A-BD67BF18B2A5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-4110" windowWidth="19440" windowHeight="15000" tabRatio="330" activeTab="1" xr2:uid="{9F6B9CB7-5928-4F67-A075-287239088E00}"/>
+    <workbookView xWindow="8055" yWindow="-15480" windowWidth="19440" windowHeight="15000" tabRatio="330" firstSheet="1" activeTab="2" xr2:uid="{9F6B9CB7-5928-4F67-A075-287239088E00}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="10k incidents - 2k words" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="163">
   <si>
     <t>Common</t>
   </si>
@@ -71,6 +72,456 @@
   </si>
   <si>
     <t>Label</t>
+  </si>
+  <si>
+    <t>Top Cenitex Words</t>
+  </si>
+  <si>
+    <t>Top Uncommon Words</t>
+  </si>
+  <si>
+    <t>Word</t>
+  </si>
+  <si>
+    <t>Times</t>
+  </si>
+  <si>
+    <t>citrix</t>
+  </si>
+  <si>
+    <t>lotus</t>
+  </si>
+  <si>
+    <t>cenitex</t>
+  </si>
+  <si>
+    <t>delwp</t>
+  </si>
+  <si>
+    <t>dpc</t>
+  </si>
+  <si>
+    <t>dtf</t>
+  </si>
+  <si>
+    <t>melbourne</t>
+  </si>
+  <si>
+    <t>victoria</t>
+  </si>
+  <si>
+    <t>remedy</t>
+  </si>
+  <si>
+    <t>depts</t>
+  </si>
+  <si>
+    <t>dedjtr</t>
+  </si>
+  <si>
+    <t>reset</t>
+  </si>
+  <si>
+    <t>confirmed</t>
+  </si>
+  <si>
+    <t>troubleshooting</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>y/n</t>
+  </si>
+  <si>
+    <t>opswiki</t>
+  </si>
+  <si>
+    <t>msc</t>
+  </si>
+  <si>
+    <t>workstation/computer</t>
+  </si>
+  <si>
+    <t>traveler</t>
+  </si>
+  <si>
+    <t>token</t>
+  </si>
+  <si>
+    <t>steps</t>
+  </si>
+  <si>
+    <t>attempt</t>
+  </si>
+  <si>
+    <t>requests</t>
+  </si>
+  <si>
+    <t>desk</t>
+  </si>
+  <si>
+    <t>mobility</t>
+  </si>
+  <si>
+    <t>approval</t>
+  </si>
+  <si>
+    <t>fault</t>
+  </si>
+  <si>
+    <t>template</t>
+  </si>
+  <si>
+    <t>screenshot</t>
+  </si>
+  <si>
+    <t>attach</t>
+  </si>
+  <si>
+    <t>chargeable</t>
+  </si>
+  <si>
+    <t>locked</t>
+  </si>
+  <si>
+    <t>requesting</t>
+  </si>
+  <si>
+    <t>confirm</t>
+  </si>
+  <si>
+    <t>resolve</t>
+  </si>
+  <si>
+    <t>incident</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>advised</t>
+  </si>
+  <si>
+    <t>folder</t>
+  </si>
+  <si>
+    <t>workplace</t>
+  </si>
+  <si>
+    <t>starter</t>
+  </si>
+  <si>
+    <t>queue</t>
+  </si>
+  <si>
+    <t>requested</t>
+  </si>
+  <si>
+    <t>moved</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>assign</t>
+  </si>
+  <si>
+    <t>refer</t>
+  </si>
+  <si>
+    <t>assisted</t>
+  </si>
+  <si>
+    <t>onboarding</t>
+  </si>
+  <si>
+    <t>packaged</t>
+  </si>
+  <si>
+    <t>logged</t>
+  </si>
+  <si>
+    <t>reboot</t>
+  </si>
+  <si>
+    <t>crg</t>
+  </si>
+  <si>
+    <t>rsa</t>
+  </si>
+  <si>
+    <t>install</t>
+  </si>
+  <si>
+    <t>gips</t>
+  </si>
+  <si>
+    <t>unable</t>
+  </si>
+  <si>
+    <t>regards</t>
+  </si>
+  <si>
+    <t>embedded</t>
+  </si>
+  <si>
+    <t>resolved</t>
+  </si>
+  <si>
+    <t>emails</t>
+  </si>
+  <si>
+    <t>worklog</t>
+  </si>
+  <si>
+    <t>cannot</t>
+  </si>
+  <si>
+    <t>affected</t>
+  </si>
+  <si>
+    <t>iphone</t>
+  </si>
+  <si>
+    <t>1/2</t>
+  </si>
+  <si>
+    <t>acctadmin</t>
+  </si>
+  <si>
+    <t>shared</t>
+  </si>
+  <si>
+    <t>approvals</t>
+  </si>
+  <si>
+    <t>accessing</t>
+  </si>
+  <si>
+    <t>severity</t>
+  </si>
+  <si>
+    <t>preapproved</t>
+  </si>
+  <si>
+    <t>passwords</t>
+  </si>
+  <si>
+    <t>departmental</t>
+  </si>
+  <si>
+    <t>lachlan</t>
+  </si>
+  <si>
+    <t>colleague</t>
+  </si>
+  <si>
+    <t>replacement</t>
+  </si>
+  <si>
+    <t>trim</t>
+  </si>
+  <si>
+    <t>occurs</t>
+  </si>
+  <si>
+    <t>wss</t>
+  </si>
+  <si>
+    <t>luise</t>
+  </si>
+  <si>
+    <t>ptv</t>
+  </si>
+  <si>
+    <t>unlock</t>
+  </si>
+  <si>
+    <t>persson</t>
+  </si>
+  <si>
+    <t>mccubbin</t>
+  </si>
+  <si>
+    <t>setup</t>
+  </si>
+  <si>
+    <t>fixing</t>
+  </si>
+  <si>
+    <t>tyson</t>
+  </si>
+  <si>
+    <t>ramon</t>
+  </si>
+  <si>
+    <t>zoran</t>
+  </si>
+  <si>
+    <t>brzakovic</t>
+  </si>
+  <si>
+    <t>oba</t>
+  </si>
+  <si>
+    <t>visio</t>
+  </si>
+  <si>
+    <t>3000</t>
+  </si>
+  <si>
+    <t>describe</t>
+  </si>
+  <si>
+    <t>smartphone</t>
+  </si>
+  <si>
+    <t>tested</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>relate</t>
+  </si>
+  <si>
+    <t>vdi</t>
+  </si>
+  <si>
+    <t>queries</t>
+  </si>
+  <si>
+    <t>hr</t>
+  </si>
+  <si>
+    <t>computer/laptop</t>
+  </si>
+  <si>
+    <t>advise</t>
+  </si>
+  <si>
+    <t>hesitate</t>
+  </si>
+  <si>
+    <t>constantly</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>fails</t>
+  </si>
+  <si>
+    <t>deleted</t>
+  </si>
+  <si>
+    <t>missing</t>
+  </si>
+  <si>
+    <t>mailbox</t>
+  </si>
+  <si>
+    <t>seek</t>
+  </si>
+  <si>
+    <t>locking</t>
+  </si>
+  <si>
+    <t>restore</t>
+  </si>
+  <si>
+    <t>consistently</t>
+  </si>
+  <si>
+    <t>unlocked</t>
+  </si>
+  <si>
+    <t>"network</t>
+  </si>
+  <si>
+    <t>out"</t>
+  </si>
+  <si>
+    <t>1800</t>
+  </si>
+  <si>
+    <t>restart</t>
+  </si>
+  <si>
+    <t>query</t>
+  </si>
+  <si>
+    <t>attached</t>
+  </si>
+  <si>
+    <t>plug</t>
+  </si>
+  <si>
+    <t>emailed</t>
+  </si>
+  <si>
+    <t>assigning</t>
+  </si>
+  <si>
+    <t>checked</t>
+  </si>
+  <si>
+    <t>8392</t>
+  </si>
+  <si>
+    <t>%msc%</t>
+  </si>
+  <si>
+    <t>populated</t>
+  </si>
+  <si>
+    <t>credentials</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>helps</t>
+  </si>
+  <si>
+    <t>replication</t>
+  </si>
+  <si>
+    <t>ticket</t>
+  </si>
+  <si>
+    <t>circumstances</t>
+  </si>
+  <si>
+    <t>cio</t>
+  </si>
+  <si>
+    <t>successfully</t>
+  </si>
+  <si>
+    <t>expiry</t>
+  </si>
+  <si>
+    <t>configuration</t>
+  </si>
+  <si>
+    <t>accessed</t>
+  </si>
+  <si>
+    <t>launching</t>
+  </si>
+  <si>
+    <t>reinstall</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>encounter</t>
+  </si>
+  <si>
+    <t>domino</t>
   </si>
 </sst>
 </file>
@@ -166,7 +617,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -199,20 +650,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="10" fontId="2" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1794,26 +2256,26 @@
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="20" t="s">
+      <c r="E1" s="21"/>
+      <c r="F1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="20"/>
-      <c r="H1" s="19" t="s">
+      <c r="G1" s="23"/>
+      <c r="H1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="19"/>
-      <c r="J1" s="20" t="s">
+      <c r="I1" s="21"/>
+      <c r="J1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="20"/>
-      <c r="L1" s="19" t="s">
+      <c r="K1" s="23"/>
+      <c r="L1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="19"/>
+      <c r="M1" s="21"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
@@ -1855,7 +2317,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="22" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="7" t="str">
@@ -1894,7 +2356,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="7" t="str">
         <f>A$3&amp;" Inc (NC)"</f>
         <v>1k Inc (NC)</v>
@@ -1931,7 +2393,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="22" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="7" t="str">
@@ -1970,7 +2432,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="7" t="str">
         <f>A$5&amp;" Inc (NC)"</f>
         <v>2k Inc (NC)</v>
@@ -2007,7 +2469,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="22" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="7" t="str">
@@ -2046,7 +2508,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="7" t="str">
         <f>A$7&amp;" Inc (NC)"</f>
         <v>5k Inc (NC)</v>
@@ -2083,7 +2545,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="22" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="7" t="str">
@@ -2122,7 +2584,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="7" t="str">
         <f>A$9&amp;" Inc (NC)"</f>
         <v>10k Inc (NC)</v>
@@ -2159,7 +2621,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="22" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="7" t="str">
@@ -2198,7 +2660,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="7" t="str">
         <f>A$11&amp;" Inc (NC)"</f>
         <v>20k Inc (NC)</v>
@@ -2235,7 +2697,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="22" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="7" t="str">
@@ -2274,7 +2736,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
+      <c r="A14" s="22"/>
       <c r="B14" s="7" t="str">
         <f>A$13&amp;" Inc (NC)"</f>
         <v>50k Inc (NC)</v>
@@ -2311,7 +2773,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="22" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="7" t="str">
@@ -2350,7 +2812,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="7" t="str">
         <f>A$15&amp;" Inc (NC)"</f>
         <v>100k Inc (NC)</v>
@@ -2489,7 +2951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32844F55-7C7E-4805-B0B9-974AE66C65D5}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -2507,7 +2969,7 @@
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="18" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2515,10 +2977,10 @@
       <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="23">
+      <c r="B2" s="20">
         <v>0.89464727722772275</v>
       </c>
-      <c r="C2" s="22">
+      <c r="C2" s="19">
         <v>0.10535272277227722</v>
       </c>
     </row>
@@ -2526,10 +2988,10 @@
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="20">
         <v>0.92582524271844657</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="19">
         <v>7.41747572815534E-2</v>
       </c>
     </row>
@@ -2537,10 +2999,10 @@
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="23">
+      <c r="B4" s="20">
         <v>0.95620671283963776</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="19">
         <v>4.3793287160362279E-2</v>
       </c>
     </row>
@@ -2548,10 +3010,10 @@
       <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="23">
+      <c r="B5" s="20">
         <v>0.97182507664999196</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="19">
         <v>2.8174923350008069E-2</v>
       </c>
     </row>
@@ -2559,10 +3021,10 @@
       <c r="A6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="23">
+      <c r="B6" s="20">
         <v>0.98109585611150518</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="19">
         <v>1.8904143888494762E-2</v>
       </c>
     </row>
@@ -2570,10 +3032,10 @@
       <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="23">
+      <c r="B7" s="20">
         <v>0.9896887138482845</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="19">
         <v>1.0311286151715482E-2</v>
       </c>
     </row>
@@ -2581,10 +3043,10 @@
       <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="23">
+      <c r="B8" s="20">
         <v>0.99334061060421941</v>
       </c>
-      <c r="C8" s="22">
+      <c r="C8" s="19">
         <v>6.6593893957805558E-3</v>
       </c>
     </row>
@@ -2593,4 +3055,1200 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED69CB3-0F1C-4D7A-9E2A-3FE04279014F}">
+  <dimension ref="A1:E137"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="27" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="D1" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="25"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="27">
+        <v>4767</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="27">
+        <v>12432</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="27">
+        <v>4381</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="27">
+        <v>6541</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="27">
+        <v>4341</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="27">
+        <v>5497</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="27">
+        <v>2788</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="27">
+        <v>4818</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="27">
+        <v>2567</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="27">
+        <v>4539</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="27">
+        <v>1607</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="27">
+        <v>4015</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="27">
+        <v>1408</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="27">
+        <v>3536</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="27">
+        <v>1383</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="27">
+        <v>3384</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="27">
+        <v>1283</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="27">
+        <v>3358</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="27">
+        <v>963</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="27">
+        <v>3128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="27">
+        <v>772</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="27">
+        <v>3114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="27">
+        <v>2940</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="27">
+        <v>2848</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="27">
+        <v>2746</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="27">
+        <v>2668</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="27">
+        <v>2584</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="27">
+        <v>2481</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D20" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="27">
+        <v>2479</v>
+      </c>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D21" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="27">
+        <v>2451</v>
+      </c>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D22" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" s="27">
+        <v>2238</v>
+      </c>
+    </row>
+    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D23" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="27">
+        <v>2095</v>
+      </c>
+    </row>
+    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D24" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="27">
+        <v>1895</v>
+      </c>
+    </row>
+    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D25" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" s="27">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D26" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" s="27">
+        <v>1753</v>
+      </c>
+    </row>
+    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D27" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="27">
+        <v>1724</v>
+      </c>
+    </row>
+    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D28" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" s="27">
+        <v>1721</v>
+      </c>
+    </row>
+    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D29" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="E29" s="27">
+        <v>1665</v>
+      </c>
+    </row>
+    <row r="30" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D30" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30" s="27">
+        <v>1658</v>
+      </c>
+    </row>
+    <row r="31" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D31" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E31" s="27">
+        <v>1577</v>
+      </c>
+    </row>
+    <row r="32" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D32" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="E32" s="27">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D33" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" s="27">
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D34" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34" s="27">
+        <v>1498</v>
+      </c>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D35" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E35" s="27">
+        <v>1463</v>
+      </c>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D36" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E36" s="27">
+        <v>1447</v>
+      </c>
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D37" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="E37" s="27">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D38" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="E38" s="27">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D39" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="E39" s="27">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="40" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D40" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="E40" s="27">
+        <v>1409</v>
+      </c>
+    </row>
+    <row r="41" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D41" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="E41" s="27">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="42" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D42" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="E42" s="27">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="43" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D43" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="E43" s="27">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="44" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D44" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E44" s="27">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="45" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D45" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E45" s="27">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="46" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D46" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="E46" s="27">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="47" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D47" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E47" s="27">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="48" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D48" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E48" s="27">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D49" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="E49" s="27">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="50" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D50" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="E50" s="27">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="51" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D51" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E51" s="27">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="52" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D52" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="E52" s="27">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="53" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D53" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="E53" s="27">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="54" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D54" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="E54" s="27">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="55" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D55" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="E55" s="27">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="56" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D56" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="E56" s="27">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="57" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D57" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E57" s="27">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="58" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D58" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="E58" s="27">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="59" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D59" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="E59" s="27">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="60" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D60" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="E60" s="27">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="61" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D61" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="E61" s="27">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="62" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D62" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="E62" s="27">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="63" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D63" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="E63" s="27">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="64" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D64" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="E64" s="27">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="65" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D65" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="E65" s="27">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="66" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D66" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="E66" s="27">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="67" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D67" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="E67" s="27">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="68" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D68" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="E68" s="27">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="69" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D69" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="E69" s="27">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="70" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D70" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="E70" s="27">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="71" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D71" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="E71" s="27">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="72" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D72" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="E72" s="27">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="73" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D73" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="E73" s="27">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="74" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D74" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="E74" s="27">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="75" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D75" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="E75" s="27">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="76" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D76" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="E76" s="27">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="77" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D77" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="E77" s="27">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="78" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D78" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="E78" s="27">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="79" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D79" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="E79" s="27">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="80" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D80" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="E80" s="27">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="81" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D81" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="E81" s="27">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="82" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D82" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="E82" s="27">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="83" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D83" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="E83" s="27">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="84" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D84" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="E84" s="27">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="85" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D85" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="E85" s="27">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="86" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D86" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="E86" s="27">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="87" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D87" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="E87" s="27">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="88" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D88" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="E88" s="27">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="89" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D89" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="E89" s="27">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="90" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D90" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E90" s="27">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="91" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D91" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E91" s="27">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="92" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D92" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="E92" s="27">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="93" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D93" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="E93" s="27">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="94" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D94" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="E94" s="27">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="95" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D95" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="E95" s="27">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="96" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D96" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="E96" s="27">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="97" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D97" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="E97" s="27">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="98" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D98" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="E98" s="27">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="99" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D99" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="E99" s="27">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="100" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D100" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="E100" s="27">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="101" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D101" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="E101" s="27">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="102" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D102" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="E102" s="27">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="103" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D103" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="E103" s="27">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="104" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D104" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="E104" s="27">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="105" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D105" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="E105" s="27">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="106" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D106" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="E106" s="27">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="107" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D107" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="E107" s="27">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="108" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D108" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="E108" s="27">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="109" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D109" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="E109" s="27">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="110" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D110" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E110" s="27">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="111" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D111" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="E111" s="27">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="112" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D112" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="E112" s="27">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="113" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D113" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="E113" s="27">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="114" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D114" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="E114" s="27">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="115" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D115" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="E115" s="27">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="116" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D116" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="E116" s="27">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="117" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D117" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="E117" s="27">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="118" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D118" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="E118" s="27">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="119" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D119" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="E119" s="27">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="120" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D120" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="E120" s="27">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="121" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D121" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="E121" s="27">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="122" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D122" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="E122" s="27">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="123" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D123" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="E123" s="27">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="124" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D124" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="E124" s="27">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="125" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D125" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="E125" s="27">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="126" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D126" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="E126" s="27">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="127" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D127" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="E127" s="27">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="128" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D128" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="E128" s="27">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="129" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D129" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="E129" s="27">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="130" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D130" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="E130" s="27">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="131" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D131" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="E131" s="27">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="132" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D132" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="E132" s="27">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="133" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D133" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="E133" s="27">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="134" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D134" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="E134" s="27">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="135" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D135" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="E135" s="27">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="136" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D136" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="E136" s="27">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="137" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D137" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="E137" s="27">
+        <v>470</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>